<commit_message>
Changes done for excel updation
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC28_Verify_PunchOut_User.xlsx
+++ b/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC28_Verify_PunchOut_User.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Actual_testcases\Kaman\ECTEST\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2041F2DA-F9C0-459B-BBA7-24C43E776629}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD19EC7-11CC-42FB-9DAF-70344DB86978}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TC28_Verify_PunchOut_User" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
   <si>
     <t>TestCase</t>
   </si>
@@ -103,19 +103,7 @@
     <t>CSS</t>
   </si>
   <si>
-    <t>CLICK_JS</t>
-  </si>
-  <si>
-    <t>EnableCertificate_MoreInfo</t>
-  </si>
-  <si>
-    <t>JS_ID</t>
-  </si>
-  <si>
     <t>EleType1</t>
-  </si>
-  <si>
-    <t>EnableCertificate_GoTOPage</t>
   </si>
   <si>
     <t>EleType2</t>
@@ -561,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -615,100 +603,100 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
+    <row r="4" spans="1:5">
       <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
-        <v>24</v>
+      <c r="B4" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1">
+        <v>28</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1">
+        <v>29</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1">
+      <c r="D6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="3"/>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="4"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1">
+    <row r="8" spans="1:5">
       <c r="A8" s="3"/>
-      <c r="B8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="3"/>
+      <c r="B8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="4"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="3"/>
-      <c r="B10" s="3" t="s">
-        <v>33</v>
+      <c r="B10" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>34</v>
-      </c>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="3"/>
-      <c r="B11" s="3" t="s">
-        <v>35</v>
+      <c r="B11" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E11" s="3"/>
@@ -716,81 +704,24 @@
     <row r="12" spans="1:5">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="3"/>
-      <c r="B13" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="4"/>
+      <c r="B13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -805,7 +736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -852,31 +783,31 @@
         <v>19</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -886,12 +817,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1092,15 +1020,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1125,10 +1057,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>